<commit_message>
Update WMS Gantt Chart
</commit_message>
<xml_diff>
--- a/WMS Gantt Chart.xlsx
+++ b/WMS Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b3altena\Google Drive\College\4 - Senior\Fall 2018\COM S 329\AltenaB_Assignment_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F679F90-CB50-4BCF-94C0-212B5D78B181}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F3B40C3-766C-4600-8A06-AD605A18058D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
   <si>
     <t>Activity</t>
   </si>
@@ -58,33 +58,36 @@
     <t xml:space="preserve">            Manufacture Parts Needed</t>
   </si>
   <si>
+    <t>Drew</t>
+  </si>
+  <si>
     <t xml:space="preserve">            Develop a network connection</t>
   </si>
   <si>
+    <t xml:space="preserve">            Create interactive software application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Define user/admin privileges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Test hardware parts</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2.2 Mobile Application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Set up app layout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Establish Connection with Hardware</t>
+  </si>
+  <si>
     <t>Kristian</t>
   </si>
   <si>
-    <t xml:space="preserve">            Create interactive software application</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            Define user/admin privileges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            Test hardware parts</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    2.2 Mobile Application</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            Set up app layout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            Establish Connection with Hardware</t>
-  </si>
-  <si>
     <t xml:space="preserve">            Establish Connection with Server</t>
   </si>
   <si>
@@ -215,6 +218,9 @@
   </si>
   <si>
     <t xml:space="preserve">            Create Compression Plan</t>
+  </si>
+  <si>
+    <t>Jase, Drew</t>
   </si>
   <si>
     <t xml:space="preserve">        4.1.3 Potential Optimization Plans</t>
@@ -558,7 +564,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{270F9777-D890-402D-ABF4-842435017B46}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{FBA929C0-99E5-4FD9-A834-1694356569EC}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1077,7 +1083,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -1086,10 +1092,10 @@
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -1112,7 +1118,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
@@ -1159,7 +1165,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
@@ -1167,10 +1173,10 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -1178,7 +1184,7 @@
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>17</v>
@@ -1194,14 +1200,14 @@
     </row>
     <row r="23" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23" s="7"/>
       <c r="O23" s="8"/>
     </row>
     <row r="24" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>6</v>
@@ -1213,7 +1219,7 @@
     </row>
     <row r="25" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>6</v>
@@ -1224,7 +1230,7 @@
     </row>
     <row r="26" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>6</v>
@@ -1235,7 +1241,7 @@
     </row>
     <row r="27" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>6</v>
@@ -1252,24 +1258,24 @@
     </row>
     <row r="29" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="7"/>
       <c r="O29" s="8"/>
     </row>
     <row r="30" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="7"/>
       <c r="O30" s="8"/>
     </row>
     <row r="31" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
@@ -1278,10 +1284,10 @@
     </row>
     <row r="32" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
@@ -1290,10 +1296,10 @@
     </row>
     <row r="33" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
@@ -1302,10 +1308,10 @@
     </row>
     <row r="34" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="K34" s="14"/>
       <c r="L34" s="14"/>
@@ -1313,7 +1319,7 @@
     </row>
     <row r="35" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>6</v>
@@ -1329,14 +1335,14 @@
     </row>
     <row r="37" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B37" s="7"/>
       <c r="O37" s="8"/>
     </row>
     <row r="38" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>10</v>
@@ -1347,7 +1353,7 @@
     </row>
     <row r="39" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>10</v>
@@ -1360,7 +1366,7 @@
     </row>
     <row r="40" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>6</v>
@@ -1371,7 +1377,7 @@
     </row>
     <row r="41" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>10</v>
@@ -1418,7 +1424,7 @@
     </row>
     <row r="44" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="4"/>
@@ -1437,24 +1443,24 @@
     </row>
     <row r="45" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B45" s="7"/>
       <c r="O45" s="8"/>
     </row>
     <row r="46" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B46" s="7"/>
       <c r="O46" s="8"/>
     </row>
     <row r="47" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
@@ -1465,10 +1471,10 @@
     </row>
     <row r="48" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
@@ -1479,10 +1485,10 @@
     </row>
     <row r="49" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="J49" s="14"/>
       <c r="K49" s="14"/>
@@ -1491,7 +1497,7 @@
     </row>
     <row r="50" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>10</v>
@@ -1503,7 +1509,7 @@
     </row>
     <row r="51" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>17</v>
@@ -1522,14 +1528,14 @@
     </row>
     <row r="53" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B53" s="7"/>
       <c r="O53" s="8"/>
     </row>
     <row r="54" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>10</v>
@@ -1543,10 +1549,10 @@
     </row>
     <row r="55" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="J55" s="14"/>
       <c r="K55" s="14"/>
@@ -1557,7 +1563,7 @@
     </row>
     <row r="56" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>6</v>
@@ -1576,14 +1582,14 @@
     </row>
     <row r="58" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B58" s="7"/>
       <c r="O58" s="8"/>
     </row>
     <row r="59" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>17</v>
@@ -1599,21 +1605,21 @@
     </row>
     <row r="61" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B61" s="7"/>
       <c r="O61" s="8"/>
     </row>
     <row r="62" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B62" s="7"/>
       <c r="O62" s="8"/>
     </row>
     <row r="63" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>17</v>
@@ -1638,14 +1644,14 @@
     </row>
     <row r="65" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B65" s="7"/>
       <c r="O65" s="8"/>
     </row>
     <row r="66" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>17</v>
@@ -1670,14 +1676,14 @@
     </row>
     <row r="68" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B68" s="7"/>
       <c r="O68" s="8"/>
     </row>
     <row r="69" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>17</v>
@@ -1731,7 +1737,7 @@
     </row>
     <row r="72" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="4"/>
@@ -1750,21 +1756,21 @@
     </row>
     <row r="73" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B73" s="7"/>
       <c r="O73" s="8"/>
     </row>
     <row r="74" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B74" s="7"/>
       <c r="O74" s="8"/>
     </row>
     <row r="75" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>6</v>
@@ -1778,17 +1784,17 @@
     </row>
     <row r="77" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B77" s="7"/>
       <c r="O77" s="8"/>
     </row>
     <row r="78" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="O78" s="17"/>
     </row>
@@ -1799,17 +1805,17 @@
     </row>
     <row r="80" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B80" s="7"/>
       <c r="O80" s="8"/>
     </row>
     <row r="81" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>

</xml_diff>